<commit_message>
update the evaluation report.
add the ttc lidar and camera as example for AKAZE/BREIF
</commit_message>
<xml_diff>
--- a/Camera3DReport.xlsx
+++ b/Camera3DReport.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8328" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Evaluation" sheetId="1" r:id="rId1"/>
+    <sheet name="ttcLidar and ttcCamera" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
   <si>
     <t>SHITOMASI</t>
   </si>
@@ -124,6 +125,120 @@
   </si>
   <si>
     <t>10.279s</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>TTC lidar</t>
+  </si>
+  <si>
+    <t>TTC camera</t>
+  </si>
+  <si>
+    <t>12.5156s</t>
+  </si>
+  <si>
+    <t>12.614s</t>
+  </si>
+  <si>
+    <t>12.312s</t>
+  </si>
+  <si>
+    <t>14.091s</t>
+  </si>
+  <si>
+    <t>12.067s</t>
+  </si>
+  <si>
+    <t>16.689s</t>
+  </si>
+  <si>
+    <t>13.108s</t>
+  </si>
+  <si>
+    <t>15.908s</t>
+  </si>
+  <si>
+    <t>13.607s</t>
+  </si>
+  <si>
+    <t>12.67s</t>
+  </si>
+  <si>
+    <t>12.15s</t>
+  </si>
+  <si>
+    <t>12.176s</t>
+  </si>
+  <si>
+    <t>14.913s</t>
+  </si>
+  <si>
+    <t>12.901s</t>
+  </si>
+  <si>
+    <t>14.412s</t>
+  </si>
+  <si>
+    <t>13.0241s</t>
+  </si>
+  <si>
+    <t>12.464s</t>
+  </si>
+  <si>
+    <t>11.174s</t>
+  </si>
+  <si>
+    <t>11.666s</t>
+  </si>
+  <si>
+    <t>12.808s</t>
+  </si>
+  <si>
+    <t>11.397s</t>
+  </si>
+  <si>
+    <t>9.071s</t>
+  </si>
+  <si>
+    <t>10.195s</t>
+  </si>
+  <si>
+    <t>9.965s</t>
+  </si>
+  <si>
+    <t>10.107s</t>
+  </si>
+  <si>
+    <t>9.472s</t>
+  </si>
+  <si>
+    <t>10.638s</t>
+  </si>
+  <si>
+    <t>8.573s</t>
+  </si>
+  <si>
+    <t>10.269s</t>
+  </si>
+  <si>
+    <t>9.516s</t>
+  </si>
+  <si>
+    <t>10.490s</t>
+  </si>
+  <si>
+    <t>9.546s</t>
+  </si>
+  <si>
+    <t>9.187s</t>
+  </si>
+  <si>
+    <t>8.398s</t>
+  </si>
+  <si>
+    <t>8.624s</t>
   </si>
 </sst>
 </file>
@@ -173,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -196,22 +311,236 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="19">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -607,17 +936,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A46" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A46" totalsRowShown="0" headerRowDxfId="7" dataDxfId="15" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:A46"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Detector Type" dataDxfId="1"/>
+    <tableColumn id="1" name="Detector Type" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B1:B46" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B1:B46" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="14">
   <autoFilter ref="B1:B46"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Descriptor Type"/>
@@ -627,7 +956,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="C1:C46" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="C1:C46" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="12">
   <autoFilter ref="C1:C46"/>
   <tableColumns count="1">
     <tableColumn id="1" name="TTC LIDAR 1st Frame"/>
@@ -637,12 +966,24 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="D1:D46" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="D1:D46" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="10">
   <autoFilter ref="D1:D46"/>
   <tableColumns count="1">
     <tableColumn id="1" name="TTC Camera 1st Frame"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:C19" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:C19"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Frame" dataDxfId="3"/>
+    <tableColumn id="2" name="TTC lidar" dataDxfId="2"/>
+    <tableColumn id="3" name="TTC camera" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -911,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1492,4 +1833,235 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>